<commit_message>
total marks & percentage has been calculated
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -1,48 +1,440 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiexin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
+    <workbookView windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths </t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>total marks</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -50,24 +442,328 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -116,7 +812,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -151,7 +847,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,23 +1021,139 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="6" max="6" width="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2">
+        <f>SUM(B2,C2,D2)</f>
+        <v>125</v>
+      </c>
+      <c r="F2" s="3">
+        <f>E2/$K$3*100</f>
+        <v>41.6666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2">
+        <v>89</v>
+      </c>
+      <c r="D3" s="2">
+        <v>81</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(B3,C3,D3)</f>
+        <v>248</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3/$K$3*100</f>
+        <v>82.6666666666667</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2">
+        <v>76</v>
+      </c>
+      <c r="D4" s="2">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2">
+        <f>SUM(B4,C4,D4)</f>
+        <v>244</v>
+      </c>
+      <c r="F4" s="3">
+        <f>E4/$K$3*100</f>
+        <v>81.3333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2">
+        <v>66</v>
+      </c>
+      <c r="D5" s="2">
+        <v>78</v>
+      </c>
+      <c r="E5" s="2">
+        <f>SUM(B5,C5,D5)</f>
+        <v>211</v>
+      </c>
+      <c r="F5" s="3">
+        <f>E5/$K$3*100</f>
+        <v>70.3333333333333</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>